<commit_message>
Fixed bugs, added sample plots
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile.xlsx
@@ -160,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +170,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -197,10 +206,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +494,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +522,7 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -520,7 +530,7 @@
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -528,7 +538,7 @@
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -539,10 +549,10 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -553,10 +563,10 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -567,10 +577,10 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -581,10 +591,10 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -595,10 +605,10 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -606,7 +616,7 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -614,7 +624,7 @@
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -622,7 +632,7 @@
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -633,10 +643,10 @@
       <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -644,7 +654,7 @@
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -652,7 +662,7 @@
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -660,7 +670,7 @@
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>